<commit_message>
Sd integration jdv r5 (#55)
* ajout CS et VS title type ebb5c2d0c8713d63875c90dfcef28895f0d16c11
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-label.xlsx
+++ b/ig/main/StructureDefinition-eclaire-label.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-01T08:48:57+00:00</t>
+    <t>2023-09-01T14:26:19+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -267,7 +267,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/title-type</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-study-title-type-vs</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -630,7 +630,7 @@
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="34.57421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="73.859375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="10.26171875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>